<commit_message>
ajuste a plantilla excel de BO
</commit_message>
<xml_diff>
--- a/public/assets/plantillas_excel/Mod_01/SIZ_bo.xlsx
+++ b/public/assets/plantillas_excel/Mod_01/SIZ_bo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beto/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/htdocs/sizb/public/assets/plantillas_excel/Mod_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02DBA03-CAFB-6B42-AACF-B7F70368F35F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17BE819-3F80-4C46-853E-E831DFB77846}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,6 +44,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">Vicente Cueva Ramirez:
 Elaborado el 14 de Noviembre del 2014.
@@ -73,6 +74,7 @@
         <sz val="14"/>
         <color rgb="FF0000CC"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>(V160412)</t>
     </r>
@@ -411,7 +413,7 @@
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -421,67 +423,91 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF0000CC"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +532,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9BBB59"/>
+        <bgColor rgb="FF9BBB59"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FF9BBB59"/>
       </patternFill>
     </fill>
@@ -678,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -894,13 +926,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -913,6 +945,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1309,9 +1344,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1342,43 +1377,43 @@
     <col min="26" max="26" width="7.33203125" customWidth="1"/>
     <col min="27" max="27" width="8.5" customWidth="1"/>
     <col min="28" max="28" width="5.1640625" customWidth="1"/>
-    <col min="29" max="29" width="11.5" customWidth="1"/>
+    <col min="29" max="29" width="54.83203125" customWidth="1"/>
     <col min="30" max="30" width="3.6640625" customWidth="1"/>
     <col min="31" max="45" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -1398,36 +1433,36 @@
     </row>
     <row r="2" spans="1:45" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="76"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
+      <c r="AC2" s="77"/>
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
@@ -1447,36 +1482,36 @@
     </row>
     <row r="3" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="77"/>
+      <c r="X3" s="77"/>
+      <c r="Y3" s="77"/>
+      <c r="Z3" s="77"/>
+      <c r="AA3" s="77"/>
+      <c r="AB3" s="77"/>
+      <c r="AC3" s="77"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
@@ -1514,9 +1549,9 @@
         <f>SUBTOTAL(9,M5:M15757)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
@@ -1614,7 +1649,7 @@
       <c r="V5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="38" t="s">
+      <c r="W5" s="75" t="s">
         <v>24</v>
       </c>
       <c r="X5" s="23" t="s">

</xml_diff>